<commit_message>
add missing date and names for treatment
</commit_message>
<xml_diff>
--- a/data/management/Management_information_BON_2015.xlsx
+++ b/data/management/Management_information_BON_2015.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\data\management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F1F101-1746-4E41-B171-C842E93BDBEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BON_2015" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="183">
   <si>
     <t>General information</t>
   </si>
@@ -570,7 +576,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -896,16 +902,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
-    <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -981,6 +987,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1028,7 +1037,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1061,9 +1070,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1096,6 +1122,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1271,11 +1314,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1549,7 @@
       <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="41">
         <v>41913</v>
       </c>
       <c r="F23" s="31"/>
@@ -1610,7 +1653,7 @@
       <c r="B29" s="12">
         <v>0.15</v>
       </c>
-      <c r="C29" s="42">
+      <c r="C29" s="41">
         <v>42248</v>
       </c>
       <c r="F29" s="31"/>
@@ -1629,7 +1672,7 @@
       <c r="B30" s="12">
         <v>0.08</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="41">
         <v>42248</v>
       </c>
       <c r="F30" s="31"/>
@@ -1648,7 +1691,7 @@
       <c r="B31" s="12">
         <v>0.77</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="41">
         <v>42248</v>
       </c>
       <c r="F31" s="31"/>
@@ -1667,7 +1710,7 @@
       <c r="B32" s="10">
         <v>6.6</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="41">
         <v>42248</v>
       </c>
       <c r="F32" s="31"/>
@@ -1686,11 +1729,11 @@
       <c r="B33" s="12">
         <v>1.9E-2</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="41">
         <v>42248</v>
       </c>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="11"/>
       <c r="I33" s="6"/>
     </row>
@@ -1701,7 +1744,7 @@
       <c r="B34" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="41">
         <v>42248</v>
       </c>
       <c r="F34" s="9"/>
@@ -1716,7 +1759,7 @@
       <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="41">
         <v>42248</v>
       </c>
       <c r="F35" s="6"/>
@@ -1849,8 +1892,8 @@
       <c r="B45" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="22">
-        <v>0</v>
+      <c r="C45" s="25">
+        <v>42075</v>
       </c>
       <c r="D45" s="22">
         <v>0</v>
@@ -1885,8 +1928,8 @@
       <c r="B46" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="22">
-        <v>0</v>
+      <c r="C46" s="25">
+        <v>42109</v>
       </c>
       <c r="D46" s="22">
         <v>0</v>
@@ -1921,8 +1964,8 @@
       <c r="B47" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="22">
-        <v>0</v>
+      <c r="C47" s="23">
+        <v>42151</v>
       </c>
       <c r="D47" s="22">
         <v>0</v>
@@ -2527,7 +2570,9 @@
       <c r="A69" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="22"/>
+      <c r="B69" s="22" t="s">
+        <v>68</v>
+      </c>
       <c r="C69" s="25">
         <v>42151</v>
       </c>
@@ -2717,7 +2762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C8:U32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3184,7 +3229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>